<commit_message>
recreate myvenv & fixed readme.md
</commit_message>
<xml_diff>
--- a/receipts.xlsx
+++ b/receipts.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,6 +485,26 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2016-09-29</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>FamilyMart 麻布十番一丁目店</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>茎わかめ、ハムカツサンド、中華そば</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>512</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>